<commit_message>
A new version of Outline Effect(outline color defined as chart parameter, not judgeplane's property
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Songs/World Wide Web/Chart.xlsx
+++ b/Assets/StreamingAssets/Songs/World Wide Web/Chart.xlsx
@@ -1,27 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Xenody-master\Assets\StreamingAssets\Songs\World Wide Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07EC93A7-1496-4337-876E-DBC71FB44528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F5EE69-EB4A-448F-8A13-261BCF7F1EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
   </bookViews>
   <sheets>
-    <sheet name="planes" sheetId="1" r:id="rId1"/>
-    <sheet name="taps" sheetId="2" r:id="rId2"/>
-    <sheet name="holds" sheetId="3" r:id="rId3"/>
-    <sheet name="slides" sheetId="4" r:id="rId4"/>
-    <sheet name="flicks" sheetId="5" r:id="rId5"/>
-    <sheet name="stars" sheetId="6" r:id="rId6"/>
+    <sheet name="speed" sheetId="7" r:id="rId1"/>
+    <sheet name="color" sheetId="8" r:id="rId2"/>
+    <sheet name="plane" sheetId="1" r:id="rId3"/>
+    <sheet name="tap" sheetId="2" r:id="rId4"/>
+    <sheet name="hold" sheetId="3" r:id="rId5"/>
+    <sheet name="slide" sheetId="4" r:id="rId6"/>
+    <sheet name="flick" sheetId="5" r:id="rId7"/>
+    <sheet name="star" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">stars!$O$49:$O$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">star!$O$49:$O$51</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="33">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -133,10 +135,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>color</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>#63b8ff</t>
   </si>
   <si>
@@ -144,10 +142,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>#E0EEE0</t>
+    <t>#f0ffff</t>
   </si>
   <si>
-    <t>#f0ffff</t>
+    <t>Lcolor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ucolor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -158,7 +165,7 @@
     <numFmt numFmtId="176" formatCode="0.000"/>
     <numFmt numFmtId="177" formatCode="0.000_ "/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,12 +185,6 @@
       <sz val="11"/>
       <color rgb="FF5F5F5F"/>
       <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -209,7 +210,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -220,9 +221,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -538,2448 +536,2073 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA789EFB-BCA3-4FCA-98D4-565CD71AE543}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L98"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A9C96A9-1D89-4E37-B465-2098CA6EFD66}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>999</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75FB3F29-4751-4825-9A13-CD8F2FFC98B2}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>154.828</v>
+      </c>
+      <c r="C2" t="s">
         <v>27</v>
       </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA789EFB-BCA3-4FCA-98D4-565CD71AE543}">
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:I98"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="str">
-        <f t="shared" ref="B2:B33" si="0">VLOOKUP(A2,$I$1:$J$99,2,FALSE)</f>
-        <v>#63b8ff</v>
+      <c r="B2">
+        <v>0</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>33.420999999999999</v>
       </c>
       <c r="E2">
-        <v>33.420999999999999</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="str">
-        <f t="shared" si="0"/>
-        <v>#f0ffff</v>
+      <c r="B3">
+        <v>32.015000000000001</v>
       </c>
       <c r="C3">
-        <v>32.015000000000001</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>32.482999999999997</v>
       </c>
       <c r="E3">
-        <v>32.482999999999997</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
         <v>23</v>
       </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>#f0ffff</v>
+      <c r="B4">
+        <v>32.482999999999997</v>
       </c>
       <c r="C4">
-        <v>32.482999999999997</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>32.951000000000001</v>
       </c>
       <c r="E4">
-        <v>32.951000000000001</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
         <v>23</v>
       </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="J4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>#f0ffff</v>
+      <c r="B5">
+        <v>32.482999999999997</v>
       </c>
       <c r="C5">
-        <v>32.482999999999997</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>32.951000000000001</v>
       </c>
       <c r="E5">
-        <v>32.951000000000001</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
         <v>23</v>
       </c>
-      <c r="I5">
-        <v>4</v>
-      </c>
-      <c r="J5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L5" s="2"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>#f0ffff</v>
+      <c r="B6">
+        <v>32.951000000000001</v>
       </c>
       <c r="C6">
-        <v>32.951000000000001</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>33.420999999999999</v>
       </c>
       <c r="E6">
-        <v>33.420999999999999</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
         <v>23</v>
       </c>
-      <c r="I6">
-        <v>5</v>
-      </c>
-      <c r="J6" t="s">
-        <v>31</v>
-      </c>
-      <c r="L6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>#f0ffff</v>
+      <c r="B7">
+        <v>32.951000000000001</v>
       </c>
       <c r="C7">
-        <v>32.951000000000001</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>33.420999999999999</v>
       </c>
       <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
         <v>33.420999999999999</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7">
-        <v>6</v>
-      </c>
-      <c r="J7" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7" s="2"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>#63b8ff</v>
-      </c>
       <c r="C8">
-        <v>33.420999999999999</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>33.89</v>
       </c>
       <c r="E8">
-        <v>33.89</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
         <v>26</v>
       </c>
-      <c r="I8">
-        <v>7</v>
-      </c>
-      <c r="J8" t="s">
-        <v>31</v>
-      </c>
-      <c r="L8" s="2"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>4</v>
       </c>
-      <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>#f0ffff</v>
+      <c r="B9">
+        <v>33.420999999999999</v>
       </c>
       <c r="C9">
-        <v>33.420999999999999</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>33.89</v>
       </c>
       <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
         <v>33.89</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9" t="s">
-        <v>26</v>
-      </c>
-      <c r="I9">
-        <v>8</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L9" s="2"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>#63b8ff</v>
-      </c>
       <c r="C10">
-        <v>33.89</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>48.89</v>
       </c>
       <c r="E10">
-        <v>48.89</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
         <v>23</v>
       </c>
-      <c r="I10">
-        <v>9</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10" s="2"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
-      <c r="B11" t="str">
-        <f t="shared" si="0"/>
-        <v>#f0ffff</v>
+      <c r="B11">
+        <v>33.89</v>
       </c>
       <c r="C11">
-        <v>33.89</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>48.89</v>
       </c>
       <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
         <v>48.89</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>49.241999999999997</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
         <v>23</v>
       </c>
-      <c r="I11">
-        <v>10</v>
-      </c>
-      <c r="J11" t="s">
-        <v>31</v>
-      </c>
-      <c r="L11" s="2"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>1</v>
-      </c>
-      <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C12">
-        <v>48.89</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>49.241999999999997</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12" t="s">
-        <v>23</v>
-      </c>
-      <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4</v>
       </c>
-      <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>#f0ffff</v>
+      <c r="B13">
+        <v>48.89</v>
       </c>
       <c r="C13">
-        <v>48.89</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>49.241999999999997</v>
       </c>
       <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
         <v>49.241999999999997</v>
       </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>56.39</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
         <v>23</v>
       </c>
-      <c r="L13" s="2"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="str">
-        <f t="shared" si="0"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C14">
-        <v>49.241999999999997</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>56.39</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14" t="s">
-        <v>23</v>
-      </c>
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>4</v>
       </c>
-      <c r="B15" t="str">
-        <f t="shared" si="0"/>
-        <v>#f0ffff</v>
+      <c r="B15">
+        <v>49.241999999999997</v>
       </c>
       <c r="C15">
-        <v>49.241999999999997</v>
+        <v>1</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>56.39</v>
       </c>
       <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
         <v>56.39</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>56.741999999999997</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
         <v>23</v>
       </c>
-      <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="str">
-        <f t="shared" si="0"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C16">
-        <v>56.39</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>56.741999999999997</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>23</v>
-      </c>
-      <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>4</v>
       </c>
-      <c r="B17" t="str">
-        <f t="shared" si="0"/>
-        <v>#f0ffff</v>
+      <c r="B17">
+        <v>56.39</v>
       </c>
       <c r="C17">
-        <v>56.39</v>
+        <v>1</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>56.741999999999997</v>
       </c>
       <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
         <v>56.741999999999997</v>
       </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>62.015000000000001</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
         <v>23</v>
       </c>
-      <c r="L17" s="2"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" t="str">
-        <f t="shared" si="0"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C18">
-        <v>56.741999999999997</v>
-      </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>62.015000000000001</v>
-      </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18" t="s">
-        <v>23</v>
-      </c>
-      <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>4</v>
       </c>
-      <c r="B19" t="str">
-        <f t="shared" si="0"/>
-        <v>#f0ffff</v>
+      <c r="B19">
+        <v>56.741999999999997</v>
       </c>
       <c r="C19">
-        <v>56.741999999999997</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>62.484000000000002</v>
       </c>
       <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>62.015000000000001</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
         <v>62.484000000000002</v>
       </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>62.484000000000002</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>63.89</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
         <v>23</v>
       </c>
-      <c r="L19" s="2"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" t="str">
-        <f t="shared" si="0"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C20">
-        <v>62.015000000000001</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>62.484000000000002</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-      <c r="G20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="str">
-        <f t="shared" si="0"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C21">
-        <v>62.484000000000002</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>63.89</v>
-      </c>
-      <c r="F21">
-        <v>0</v>
-      </c>
-      <c r="G21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>5</v>
       </c>
-      <c r="B22" t="str">
-        <f t="shared" si="0"/>
-        <v>#f0ffff</v>
+      <c r="B22">
+        <v>62.015000000000001</v>
       </c>
       <c r="C22">
-        <v>62.015000000000001</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>62.484000000000002</v>
       </c>
       <c r="E22">
-        <v>62.484000000000002</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>5</v>
       </c>
-      <c r="B23" t="str">
-        <f t="shared" si="0"/>
-        <v>#f0ffff</v>
+      <c r="B23">
+        <v>62.484000000000002</v>
       </c>
       <c r="C23">
-        <v>62.484000000000002</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>62.953000000000003</v>
       </c>
       <c r="E23">
-        <v>62.953000000000003</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>5</v>
       </c>
-      <c r="B24" t="str">
-        <f t="shared" si="0"/>
-        <v>#f0ffff</v>
+      <c r="B24">
+        <v>62.953000000000003</v>
       </c>
       <c r="C24">
-        <v>62.953000000000003</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>63.304000000000002</v>
       </c>
       <c r="E24">
-        <v>63.304000000000002</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>6</v>
       </c>
-      <c r="B25" t="str">
-        <f t="shared" si="0"/>
-        <v>#f0ffff</v>
+      <c r="B25">
+        <v>62.484000000000002</v>
       </c>
       <c r="C25">
-        <v>62.484000000000002</v>
+        <v>1</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>62.953000000000003</v>
       </c>
       <c r="E25">
-        <v>62.953000000000003</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>6</v>
       </c>
-      <c r="B26" t="str">
-        <f t="shared" si="0"/>
-        <v>#f0ffff</v>
+      <c r="B26">
+        <v>62.953000000000003</v>
       </c>
       <c r="C26">
-        <v>62.953000000000003</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>63.304000000000002</v>
       </c>
       <c r="E26">
-        <v>63.304000000000002</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-      <c r="G26" t="s">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
-      <c r="B27" t="str">
-        <f t="shared" si="0"/>
-        <v>#63b8ff</v>
+      <c r="B27">
+        <v>63.89</v>
       </c>
       <c r="C27">
-        <v>63.89</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>64.358999999999995</v>
       </c>
       <c r="E27">
+        <v>0.6</v>
+      </c>
+      <c r="F27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
         <v>64.358999999999995</v>
       </c>
-      <c r="F27">
+      <c r="C28">
         <v>0.6</v>
       </c>
-      <c r="G27" t="s">
+      <c r="D28">
+        <v>65.765000000000001</v>
+      </c>
+      <c r="E28">
+        <v>0.2</v>
+      </c>
+      <c r="F28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" t="str">
-        <f t="shared" si="0"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C28">
-        <v>64.358999999999995</v>
-      </c>
-      <c r="D28">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>65.765000000000001</v>
+      </c>
+      <c r="C29">
+        <v>0.2</v>
+      </c>
+      <c r="D29">
+        <v>66.233999999999995</v>
+      </c>
+      <c r="E29">
+        <v>0.8</v>
+      </c>
+      <c r="F29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>66.233999999999995</v>
+      </c>
+      <c r="C30">
+        <v>0.8</v>
+      </c>
+      <c r="D30">
+        <v>67.64</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>67.64</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>68.108999999999995</v>
+      </c>
+      <c r="E31">
         <v>0.6</v>
       </c>
-      <c r="E28">
-        <v>65.765000000000001</v>
-      </c>
-      <c r="F28">
+      <c r="F31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>68.108999999999995</v>
+      </c>
+      <c r="C32">
+        <v>0.6</v>
+      </c>
+      <c r="D32">
+        <v>69.515000000000001</v>
+      </c>
+      <c r="E32">
         <v>0.2</v>
       </c>
-      <c r="G28" t="s">
+      <c r="F32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>1</v>
-      </c>
-      <c r="B29" t="str">
-        <f t="shared" si="0"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C29">
-        <v>65.765000000000001</v>
-      </c>
-      <c r="D29">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>69.515000000000001</v>
+      </c>
+      <c r="C33">
         <v>0.2</v>
       </c>
-      <c r="E29">
-        <v>66.233999999999995</v>
-      </c>
-      <c r="F29">
+      <c r="D33">
+        <v>69.983999999999995</v>
+      </c>
+      <c r="E33">
         <v>0.8</v>
       </c>
-      <c r="G29" t="s">
+      <c r="F33" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>1</v>
-      </c>
-      <c r="B30" t="str">
-        <f t="shared" si="0"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C30">
-        <v>66.233999999999995</v>
-      </c>
-      <c r="D30">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>69.983999999999995</v>
+      </c>
+      <c r="C34">
         <v>0.8</v>
       </c>
-      <c r="E30">
-        <v>67.64</v>
-      </c>
-      <c r="F30">
-        <v>0</v>
-      </c>
-      <c r="G30" t="s">
+      <c r="D34">
+        <v>71.39</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>1</v>
-      </c>
-      <c r="B31" t="str">
-        <f t="shared" si="0"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C31">
-        <v>67.64</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>68.108999999999995</v>
-      </c>
-      <c r="F31">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>71.39</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>71.858999999999995</v>
+      </c>
+      <c r="E35">
         <v>0.6</v>
       </c>
-      <c r="G31" t="s">
+      <c r="F35" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>1</v>
-      </c>
-      <c r="B32" t="str">
-        <f t="shared" si="0"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C32">
-        <v>68.108999999999995</v>
-      </c>
-      <c r="D32">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>71.858999999999995</v>
+      </c>
+      <c r="C36">
         <v>0.6</v>
       </c>
-      <c r="E32">
-        <v>69.515000000000001</v>
-      </c>
-      <c r="F32">
+      <c r="D36">
+        <v>73.265000000000001</v>
+      </c>
+      <c r="E36">
         <v>0.2</v>
       </c>
-      <c r="G32" t="s">
+      <c r="F36" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>1</v>
-      </c>
-      <c r="B33" t="str">
-        <f t="shared" si="0"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C33">
-        <v>69.515000000000001</v>
-      </c>
-      <c r="D33">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>73.265000000000001</v>
+      </c>
+      <c r="C37">
         <v>0.2</v>
       </c>
-      <c r="E33">
-        <v>69.983999999999995</v>
-      </c>
-      <c r="F33">
+      <c r="D37">
+        <v>73.733999999999995</v>
+      </c>
+      <c r="E37">
         <v>0.8</v>
       </c>
-      <c r="G33" t="s">
+      <c r="F37" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>1</v>
-      </c>
-      <c r="B34" t="str">
-        <f t="shared" ref="B34:B65" si="1">VLOOKUP(A34,$I$1:$J$99,2,FALSE)</f>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C34">
-        <v>69.983999999999995</v>
-      </c>
-      <c r="D34">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>73.733999999999995</v>
+      </c>
+      <c r="C38">
         <v>0.8</v>
       </c>
-      <c r="E34">
-        <v>71.39</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-      <c r="G34" t="s">
+      <c r="D38">
+        <v>75.14</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>1</v>
-      </c>
-      <c r="B35" t="str">
-        <f t="shared" si="1"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C35">
-        <v>71.39</v>
-      </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>71.858999999999995</v>
-      </c>
-      <c r="F35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>75.14</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>75.608999999999995</v>
+      </c>
+      <c r="E39">
         <v>0.6</v>
       </c>
-      <c r="G35" t="s">
+      <c r="F39" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>1</v>
-      </c>
-      <c r="B36" t="str">
-        <f t="shared" si="1"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C36">
-        <v>71.858999999999995</v>
-      </c>
-      <c r="D36">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>75.608999999999995</v>
+      </c>
+      <c r="C40">
         <v>0.6</v>
       </c>
-      <c r="E36">
-        <v>73.265000000000001</v>
-      </c>
-      <c r="F36">
-        <v>0.2</v>
-      </c>
-      <c r="G36" t="s">
+      <c r="D40">
+        <v>77.015000000000001</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="B37" t="str">
-        <f t="shared" si="1"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C37">
-        <v>73.265000000000001</v>
-      </c>
-      <c r="D37">
-        <v>0.2</v>
-      </c>
-      <c r="E37">
-        <v>73.733999999999995</v>
-      </c>
-      <c r="F37">
-        <v>0.8</v>
-      </c>
-      <c r="G37" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>77.015000000000001</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>78.89</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="B38" t="str">
-        <f t="shared" si="1"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C38">
-        <v>73.733999999999995</v>
-      </c>
-      <c r="D38">
-        <v>0.8</v>
-      </c>
-      <c r="E38">
-        <v>75.14</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-      <c r="G38" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <v>78.89</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>79.358999999999995</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>1</v>
-      </c>
-      <c r="B39" t="str">
-        <f t="shared" si="1"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C39">
-        <v>75.14</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39">
-        <v>75.608999999999995</v>
-      </c>
-      <c r="F39">
-        <v>0.6</v>
-      </c>
-      <c r="G39" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="B40" t="str">
-        <f t="shared" si="1"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C40">
-        <v>75.608999999999995</v>
-      </c>
-      <c r="D40">
-        <v>0.6</v>
-      </c>
-      <c r="E40">
-        <v>77.015000000000001</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>1</v>
-      </c>
-      <c r="B41" t="str">
-        <f t="shared" si="1"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C41">
-        <v>77.015000000000001</v>
-      </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>78.89</v>
-      </c>
-      <c r="F41">
-        <v>0</v>
-      </c>
-      <c r="G41" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>1</v>
-      </c>
-      <c r="B42" t="str">
-        <f t="shared" si="1"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C42">
-        <v>78.89</v>
-      </c>
-      <c r="D42">
-        <v>0</v>
-      </c>
-      <c r="E42">
-        <v>79.358999999999995</v>
-      </c>
-      <c r="F42">
-        <v>1</v>
-      </c>
-      <c r="G42" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>7</v>
       </c>
-      <c r="B43" t="str">
-        <f t="shared" si="1"/>
-        <v>#f0ffff</v>
+      <c r="B43">
+        <v>78.89</v>
       </c>
       <c r="C43">
-        <v>78.89</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>79.358999999999995</v>
       </c>
       <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44">
         <v>79.358999999999995</v>
       </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43" t="s">
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>80.765000000000001</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>1</v>
-      </c>
-      <c r="B44" t="str">
-        <f t="shared" si="1"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C44">
-        <v>79.358999999999995</v>
-      </c>
-      <c r="D44">
-        <v>1</v>
-      </c>
-      <c r="E44">
-        <v>80.765000000000001</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>7</v>
       </c>
-      <c r="B45" t="str">
-        <f t="shared" si="1"/>
-        <v>#f0ffff</v>
+      <c r="B45">
+        <v>79.358999999999995</v>
       </c>
       <c r="C45">
-        <v>79.358999999999995</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>80.765000000000001</v>
       </c>
       <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46">
         <v>80.765000000000001</v>
       </c>
-      <c r="F45">
-        <v>1</v>
-      </c>
-      <c r="G45" t="s">
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>81.233999999999995</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>1</v>
-      </c>
-      <c r="B46" t="str">
-        <f t="shared" si="1"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C46">
-        <v>80.765000000000001</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>81.233999999999995</v>
-      </c>
-      <c r="F46">
-        <v>1</v>
-      </c>
-      <c r="G46" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>7</v>
       </c>
-      <c r="B47" t="str">
-        <f t="shared" si="1"/>
-        <v>#f0ffff</v>
+      <c r="B47">
+        <v>80.765000000000001</v>
       </c>
       <c r="C47">
-        <v>80.765000000000001</v>
+        <v>1</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>81.233999999999995</v>
       </c>
       <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48">
         <v>81.233999999999995</v>
       </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-      <c r="G47" t="s">
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>82.64</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>1</v>
-      </c>
-      <c r="B48" t="str">
-        <f t="shared" si="1"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C48">
-        <v>81.233999999999995</v>
-      </c>
-      <c r="D48">
-        <v>1</v>
-      </c>
-      <c r="E48">
-        <v>82.64</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-      <c r="G48" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>7</v>
       </c>
-      <c r="B49" t="str">
-        <f t="shared" si="1"/>
-        <v>#f0ffff</v>
+      <c r="B49">
+        <v>81.233999999999995</v>
       </c>
       <c r="C49">
-        <v>81.233999999999995</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>82.64</v>
       </c>
       <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50">
         <v>82.64</v>
       </c>
-      <c r="F49">
-        <v>1</v>
-      </c>
-      <c r="G49" t="s">
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>83.108999999999995</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>1</v>
-      </c>
-      <c r="B50" t="str">
-        <f t="shared" si="1"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C50">
-        <v>82.64</v>
-      </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="E50">
-        <v>83.108999999999995</v>
-      </c>
-      <c r="F50">
-        <v>1</v>
-      </c>
-      <c r="G50" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>7</v>
       </c>
-      <c r="B51" t="str">
-        <f t="shared" si="1"/>
-        <v>#f0ffff</v>
+      <c r="B51">
+        <v>82.64</v>
       </c>
       <c r="C51">
-        <v>82.64</v>
+        <v>1</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>83.108999999999995</v>
       </c>
       <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52">
         <v>83.108999999999995</v>
       </c>
-      <c r="F51">
-        <v>0</v>
-      </c>
-      <c r="G51" t="s">
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>84.515000000000001</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>1</v>
-      </c>
-      <c r="B52" t="str">
-        <f t="shared" si="1"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C52">
-        <v>83.108999999999995</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-      <c r="E52">
-        <v>84.515000000000001</v>
-      </c>
-      <c r="F52">
-        <v>0</v>
-      </c>
-      <c r="G52" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>7</v>
       </c>
-      <c r="B53" t="str">
-        <f t="shared" si="1"/>
-        <v>#f0ffff</v>
+      <c r="B53">
+        <v>83.108999999999995</v>
       </c>
       <c r="C53">
-        <v>83.108999999999995</v>
+        <v>0</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>84.515000000000001</v>
       </c>
       <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54">
         <v>84.515000000000001</v>
       </c>
-      <c r="F53">
-        <v>1</v>
-      </c>
-      <c r="G53" t="s">
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>84.983999999999995</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+      <c r="F54" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>1</v>
-      </c>
-      <c r="B54" t="str">
-        <f t="shared" si="1"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C54">
-        <v>84.515000000000001</v>
-      </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54">
-        <v>84.983999999999995</v>
-      </c>
-      <c r="F54">
-        <v>1</v>
-      </c>
-      <c r="G54" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>7</v>
       </c>
-      <c r="B55" t="str">
-        <f t="shared" si="1"/>
-        <v>#f0ffff</v>
+      <c r="B55">
+        <v>84.515000000000001</v>
       </c>
       <c r="C55">
-        <v>84.515000000000001</v>
+        <v>1</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>84.983999999999995</v>
       </c>
       <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56">
         <v>84.983999999999995</v>
       </c>
-      <c r="F55">
-        <v>0</v>
-      </c>
-      <c r="G55" t="s">
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>86.39</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>1</v>
-      </c>
-      <c r="B56" t="str">
-        <f t="shared" si="1"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C56">
-        <v>84.983999999999995</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-      <c r="E56">
-        <v>86.39</v>
-      </c>
-      <c r="F56">
-        <v>0</v>
-      </c>
-      <c r="G56" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>7</v>
       </c>
-      <c r="B57" t="str">
-        <f t="shared" si="1"/>
-        <v>#f0ffff</v>
+      <c r="B57">
+        <v>84.983999999999995</v>
       </c>
       <c r="C57">
-        <v>84.983999999999995</v>
+        <v>0</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>86.39</v>
       </c>
       <c r="E57">
+        <v>1</v>
+      </c>
+      <c r="F57" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58">
         <v>86.39</v>
       </c>
-      <c r="F57">
-        <v>1</v>
-      </c>
-      <c r="G57" t="s">
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>86.858999999999995</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>1</v>
-      </c>
-      <c r="B58" t="str">
-        <f t="shared" si="1"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C58">
-        <v>86.39</v>
-      </c>
-      <c r="D58">
-        <v>0</v>
-      </c>
-      <c r="E58">
-        <v>86.858999999999995</v>
-      </c>
-      <c r="F58">
-        <v>1</v>
-      </c>
-      <c r="G58" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>7</v>
       </c>
-      <c r="B59" t="str">
-        <f t="shared" si="1"/>
-        <v>#f0ffff</v>
+      <c r="B59">
+        <v>86.39</v>
       </c>
       <c r="C59">
-        <v>86.39</v>
+        <v>1</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>86.858999999999995</v>
       </c>
       <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60">
         <v>86.858999999999995</v>
       </c>
-      <c r="F59">
-        <v>0</v>
-      </c>
-      <c r="G59" t="s">
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>88.265000000000001</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>1</v>
-      </c>
-      <c r="B60" t="str">
-        <f t="shared" si="1"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C60">
-        <v>86.858999999999995</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-      <c r="E60">
-        <v>88.265000000000001</v>
-      </c>
-      <c r="F60">
-        <v>0</v>
-      </c>
-      <c r="G60" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>7</v>
       </c>
-      <c r="B61" t="str">
-        <f t="shared" si="1"/>
-        <v>#f0ffff</v>
+      <c r="B61">
+        <v>86.858999999999995</v>
       </c>
       <c r="C61">
-        <v>86.858999999999995</v>
+        <v>0</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>88.265000000000001</v>
       </c>
       <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
         <v>88.265000000000001</v>
       </c>
-      <c r="F61">
-        <v>1</v>
-      </c>
-      <c r="G61" t="s">
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>88.733999999999995</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="F62" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <v>1</v>
-      </c>
-      <c r="B62" t="str">
-        <f t="shared" si="1"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C62">
-        <v>88.265000000000001</v>
-      </c>
-      <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="E62">
-        <v>88.733999999999995</v>
-      </c>
-      <c r="F62">
-        <v>1</v>
-      </c>
-      <c r="G62" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>7</v>
       </c>
-      <c r="B63" t="str">
-        <f t="shared" si="1"/>
-        <v>#f0ffff</v>
+      <c r="B63">
+        <v>88.265000000000001</v>
       </c>
       <c r="C63">
-        <v>88.265000000000001</v>
+        <v>1</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>88.733999999999995</v>
       </c>
       <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64">
         <v>88.733999999999995</v>
       </c>
-      <c r="F63">
-        <v>0</v>
-      </c>
-      <c r="G63" t="s">
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>90.14</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>1</v>
-      </c>
-      <c r="B64" t="str">
-        <f t="shared" si="1"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C64">
-        <v>88.733999999999995</v>
-      </c>
-      <c r="D64">
-        <v>1</v>
-      </c>
-      <c r="E64">
-        <v>90.14</v>
-      </c>
-      <c r="F64">
-        <v>0</v>
-      </c>
-      <c r="G64" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>7</v>
       </c>
-      <c r="B65" t="str">
-        <f t="shared" si="1"/>
-        <v>#f0ffff</v>
+      <c r="B65">
+        <v>88.733999999999995</v>
       </c>
       <c r="C65">
-        <v>88.733999999999995</v>
+        <v>0</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>90.14</v>
       </c>
       <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="F65" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>1</v>
+      </c>
+      <c r="B66">
         <v>90.14</v>
       </c>
-      <c r="F65">
-        <v>1</v>
-      </c>
-      <c r="G65" t="s">
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>90.608999999999995</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <v>1</v>
-      </c>
-      <c r="B66" t="str">
-        <f t="shared" ref="B66:B93" si="2">VLOOKUP(A66,$I$1:$J$99,2,FALSE)</f>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C66">
-        <v>90.14</v>
-      </c>
-      <c r="D66">
-        <v>0</v>
-      </c>
-      <c r="E66">
-        <v>90.608999999999995</v>
-      </c>
-      <c r="F66">
-        <v>1</v>
-      </c>
-      <c r="G66" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>7</v>
       </c>
-      <c r="B67" t="str">
-        <f t="shared" si="2"/>
-        <v>#f0ffff</v>
+      <c r="B67">
+        <v>90.14</v>
       </c>
       <c r="C67">
-        <v>90.14</v>
+        <v>1</v>
       </c>
       <c r="D67">
-        <v>1</v>
+        <v>90.608999999999995</v>
       </c>
       <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>1</v>
+      </c>
+      <c r="B68">
         <v>90.608999999999995</v>
       </c>
-      <c r="F67">
-        <v>0</v>
-      </c>
-      <c r="G67" t="s">
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>92.015000000000001</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>1</v>
-      </c>
-      <c r="B68" t="str">
-        <f t="shared" si="2"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C68">
-        <v>90.608999999999995</v>
-      </c>
-      <c r="D68">
-        <v>1</v>
-      </c>
-      <c r="E68">
-        <v>92.015000000000001</v>
-      </c>
-      <c r="F68">
-        <v>0</v>
-      </c>
-      <c r="G68" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>7</v>
       </c>
-      <c r="B69" t="str">
-        <f t="shared" si="2"/>
-        <v>#f0ffff</v>
+      <c r="B69">
+        <v>90.608999999999995</v>
       </c>
       <c r="C69">
-        <v>90.608999999999995</v>
+        <v>0</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>92.015000000000001</v>
       </c>
       <c r="E69">
+        <v>1</v>
+      </c>
+      <c r="F69" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>1</v>
+      </c>
+      <c r="B70">
         <v>92.015000000000001</v>
       </c>
-      <c r="F69">
-        <v>1</v>
-      </c>
-      <c r="G69" t="s">
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>92.953000000000003</v>
+      </c>
+      <c r="E70">
+        <v>1</v>
+      </c>
+      <c r="F70" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>1</v>
-      </c>
-      <c r="B70" t="str">
-        <f t="shared" si="2"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C70">
-        <v>92.015000000000001</v>
-      </c>
-      <c r="D70">
-        <v>0</v>
-      </c>
-      <c r="E70">
-        <v>92.953000000000003</v>
-      </c>
-      <c r="F70">
-        <v>1</v>
-      </c>
-      <c r="G70" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>7</v>
       </c>
-      <c r="B71" t="str">
-        <f t="shared" si="2"/>
-        <v>#f0ffff</v>
+      <c r="B71">
+        <v>92.015000000000001</v>
       </c>
       <c r="C71">
-        <v>92.015000000000001</v>
+        <v>1</v>
       </c>
       <c r="D71">
-        <v>1</v>
+        <v>92.953000000000003</v>
       </c>
       <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>1</v>
+      </c>
+      <c r="B72">
         <v>92.953000000000003</v>
       </c>
-      <c r="F71">
-        <v>0</v>
-      </c>
-      <c r="G71" t="s">
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>93.421000000000006</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>1</v>
-      </c>
-      <c r="B72" t="str">
-        <f t="shared" si="2"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C72">
-        <v>92.953000000000003</v>
-      </c>
-      <c r="D72">
-        <v>1</v>
-      </c>
-      <c r="E72">
-        <v>93.421000000000006</v>
-      </c>
-      <c r="F72">
-        <v>0</v>
-      </c>
-      <c r="G72" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>7</v>
       </c>
-      <c r="B73" t="str">
-        <f t="shared" si="2"/>
-        <v>#f0ffff</v>
+      <c r="B73">
+        <v>92.953000000000003</v>
       </c>
       <c r="C73">
-        <v>92.953000000000003</v>
+        <v>0</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>93.421000000000006</v>
       </c>
       <c r="E73">
+        <v>1</v>
+      </c>
+      <c r="F73" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>1</v>
+      </c>
+      <c r="B74">
         <v>93.421000000000006</v>
       </c>
-      <c r="F73">
-        <v>1</v>
-      </c>
-      <c r="G73" t="s">
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>123.89</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>1</v>
-      </c>
-      <c r="B74" t="str">
-        <f t="shared" si="2"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C74">
-        <v>93.421000000000006</v>
-      </c>
-      <c r="D74">
-        <v>0</v>
-      </c>
-      <c r="E74">
-        <v>123.89</v>
-      </c>
-      <c r="F74">
-        <v>0</v>
-      </c>
-      <c r="G74" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>7</v>
       </c>
-      <c r="B75" t="str">
-        <f t="shared" si="2"/>
-        <v>#f0ffff</v>
+      <c r="B75">
+        <v>93.421000000000006</v>
       </c>
       <c r="C75">
-        <v>93.421000000000006</v>
+        <v>1</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>108.89</v>
       </c>
       <c r="E75">
-        <v>108.89</v>
-      </c>
-      <c r="F75">
-        <v>1</v>
-      </c>
-      <c r="G75" t="s">
+        <v>1</v>
+      </c>
+      <c r="F75" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>7</v>
       </c>
-      <c r="B76" t="str">
-        <f t="shared" si="2"/>
-        <v>#f0ffff</v>
+      <c r="B76">
+        <v>108.89</v>
       </c>
       <c r="C76">
-        <v>108.89</v>
+        <v>1</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>109.35899999999999</v>
       </c>
       <c r="E76">
-        <v>109.35899999999999</v>
-      </c>
-      <c r="F76">
-        <v>0</v>
-      </c>
-      <c r="G76" t="s">
+        <v>0</v>
+      </c>
+      <c r="F76" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>8</v>
       </c>
-      <c r="B77" t="str">
-        <f t="shared" si="2"/>
-        <v>#E0EEE0</v>
+      <c r="B77">
+        <v>107.015</v>
       </c>
       <c r="C77">
-        <v>107.015</v>
+        <v>0</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>107.48399999999999</v>
       </c>
       <c r="E77">
-        <v>107.48399999999999</v>
-      </c>
-      <c r="F77">
-        <v>1</v>
-      </c>
-      <c r="G77" t="s">
+        <v>1</v>
+      </c>
+      <c r="F77" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>8</v>
       </c>
-      <c r="B78" t="str">
-        <f t="shared" si="2"/>
-        <v>#E0EEE0</v>
+      <c r="B78">
+        <v>107.48399999999999</v>
       </c>
       <c r="C78">
-        <v>107.48399999999999</v>
+        <v>1</v>
       </c>
       <c r="D78">
-        <v>1</v>
+        <v>107.953</v>
       </c>
       <c r="E78">
-        <v>107.953</v>
-      </c>
-      <c r="F78">
-        <v>0</v>
-      </c>
-      <c r="G78" t="s">
+        <v>0</v>
+      </c>
+      <c r="F78" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>9</v>
       </c>
-      <c r="B79" t="str">
-        <f t="shared" si="2"/>
-        <v>#E0EEE0</v>
+      <c r="B79">
+        <v>107.953</v>
       </c>
       <c r="C79">
-        <v>107.953</v>
+        <v>1</v>
       </c>
       <c r="D79">
-        <v>1</v>
+        <v>108.42100000000001</v>
       </c>
       <c r="E79">
-        <v>108.42100000000001</v>
-      </c>
-      <c r="F79">
-        <v>0</v>
-      </c>
-      <c r="G79" t="s">
+        <v>0</v>
+      </c>
+      <c r="F79" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>9</v>
       </c>
-      <c r="B80" t="str">
-        <f t="shared" si="2"/>
-        <v>#E0EEE0</v>
+      <c r="B80">
+        <v>108.42100000000001</v>
       </c>
       <c r="C80">
-        <v>108.42100000000001</v>
+        <v>0</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>108.89</v>
       </c>
       <c r="E80">
-        <v>108.89</v>
-      </c>
-      <c r="F80">
-        <v>1</v>
-      </c>
-      <c r="G80" t="s">
+        <v>1</v>
+      </c>
+      <c r="F80" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>9</v>
       </c>
-      <c r="B81" t="str">
-        <f t="shared" si="2"/>
-        <v>#E0EEE0</v>
+      <c r="B81">
+        <v>108.89</v>
       </c>
       <c r="C81">
-        <v>108.89</v>
+        <v>1</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>109.35899999999999</v>
       </c>
       <c r="E81">
-        <v>109.35899999999999</v>
-      </c>
-      <c r="F81">
-        <v>0</v>
-      </c>
-      <c r="G81" t="s">
+        <v>0</v>
+      </c>
+      <c r="F81" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1</v>
       </c>
-      <c r="B82" t="str">
-        <f t="shared" si="2"/>
-        <v>#63b8ff</v>
+      <c r="B82">
+        <v>123.89</v>
       </c>
       <c r="C82">
-        <v>123.89</v>
+        <v>0</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>124.35899999999999</v>
       </c>
       <c r="E82">
+        <v>0.8</v>
+      </c>
+      <c r="F82" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>1</v>
+      </c>
+      <c r="B83">
         <v>124.35899999999999</v>
       </c>
-      <c r="F82">
+      <c r="C83">
         <v>0.8</v>
       </c>
-      <c r="G82" t="s">
+      <c r="D83">
+        <v>125.765</v>
+      </c>
+      <c r="E83">
+        <v>0.8</v>
+      </c>
+      <c r="F83" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A83">
-        <v>1</v>
-      </c>
-      <c r="B83" t="str">
-        <f t="shared" si="2"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C83">
-        <v>124.35899999999999</v>
-      </c>
-      <c r="D83">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>1</v>
+      </c>
+      <c r="B84">
+        <v>125.765</v>
+      </c>
+      <c r="C84">
         <v>0.8</v>
       </c>
-      <c r="E83">
-        <v>125.765</v>
-      </c>
-      <c r="F83">
+      <c r="D84">
+        <v>126.23399999999999</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>1</v>
+      </c>
+      <c r="B85">
+        <v>126.23399999999999</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>127.64</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>1</v>
+      </c>
+      <c r="B86">
+        <v>127.64</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>128.10900000000001</v>
+      </c>
+      <c r="E86">
         <v>0.8</v>
       </c>
-      <c r="G83" t="s">
+      <c r="F86" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A84">
-        <v>1</v>
-      </c>
-      <c r="B84" t="str">
-        <f t="shared" si="2"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C84">
-        <v>125.765</v>
-      </c>
-      <c r="D84">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>1</v>
+      </c>
+      <c r="B87">
+        <v>128.10900000000001</v>
+      </c>
+      <c r="C87">
         <v>0.8</v>
       </c>
-      <c r="E84">
-        <v>126.23399999999999</v>
-      </c>
-      <c r="F84">
-        <v>0</v>
-      </c>
-      <c r="G84" t="s">
+      <c r="D87">
+        <v>129.51499999999999</v>
+      </c>
+      <c r="E87">
+        <v>0.8</v>
+      </c>
+      <c r="F87" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A85">
-        <v>1</v>
-      </c>
-      <c r="B85" t="str">
-        <f t="shared" si="2"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C85">
-        <v>126.23399999999999</v>
-      </c>
-      <c r="D85">
-        <v>0</v>
-      </c>
-      <c r="E85">
-        <v>127.64</v>
-      </c>
-      <c r="F85">
-        <v>0</v>
-      </c>
-      <c r="G85" t="s">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>1</v>
+      </c>
+      <c r="B88">
+        <v>129.51499999999999</v>
+      </c>
+      <c r="C88">
+        <v>0.8</v>
+      </c>
+      <c r="D88">
+        <v>129.98400000000001</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A86">
-        <v>1</v>
-      </c>
-      <c r="B86" t="str">
-        <f t="shared" si="2"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C86">
-        <v>127.64</v>
-      </c>
-      <c r="D86">
-        <v>0</v>
-      </c>
-      <c r="E86">
-        <v>128.10900000000001</v>
-      </c>
-      <c r="F86">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>1</v>
+      </c>
+      <c r="B89">
+        <v>129.98400000000001</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>131.38999999999999</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>1</v>
+      </c>
+      <c r="B90">
+        <v>131.38999999999999</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>131.85900000000001</v>
+      </c>
+      <c r="E90">
         <v>0.8</v>
       </c>
-      <c r="G86" t="s">
+      <c r="F90" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>1</v>
-      </c>
-      <c r="B87" t="str">
-        <f t="shared" si="2"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C87">
-        <v>128.10900000000001</v>
-      </c>
-      <c r="D87">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>1</v>
+      </c>
+      <c r="B91">
+        <v>131.85900000000001</v>
+      </c>
+      <c r="C91">
         <v>0.8</v>
       </c>
-      <c r="E87">
-        <v>129.51499999999999</v>
-      </c>
-      <c r="F87">
+      <c r="D91">
+        <v>133.26499999999999</v>
+      </c>
+      <c r="E91">
         <v>0.8</v>
       </c>
-      <c r="G87" t="s">
+      <c r="F91" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A88">
-        <v>1</v>
-      </c>
-      <c r="B88" t="str">
-        <f t="shared" si="2"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C88">
-        <v>129.51499999999999</v>
-      </c>
-      <c r="D88">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>1</v>
+      </c>
+      <c r="B92">
+        <v>133.26499999999999</v>
+      </c>
+      <c r="C92">
         <v>0.8</v>
       </c>
-      <c r="E88">
-        <v>129.98400000000001</v>
-      </c>
-      <c r="F88">
-        <v>0</v>
-      </c>
-      <c r="G88" t="s">
+      <c r="D92">
+        <v>133.73400000000001</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A89">
-        <v>1</v>
-      </c>
-      <c r="B89" t="str">
-        <f t="shared" si="2"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C89">
-        <v>129.98400000000001</v>
-      </c>
-      <c r="D89">
-        <v>0</v>
-      </c>
-      <c r="E89">
-        <v>131.38999999999999</v>
-      </c>
-      <c r="F89">
-        <v>0</v>
-      </c>
-      <c r="G89" t="s">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>1</v>
+      </c>
+      <c r="B93">
+        <v>133.73400000000001</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>135.13999999999999</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <v>1</v>
-      </c>
-      <c r="B90" t="str">
-        <f t="shared" si="2"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C90">
-        <v>131.38999999999999</v>
-      </c>
-      <c r="D90">
-        <v>0</v>
-      </c>
-      <c r="E90">
-        <v>131.85900000000001</v>
-      </c>
-      <c r="F90">
-        <v>0.8</v>
-      </c>
-      <c r="G90" t="s">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>1</v>
+      </c>
+      <c r="B94">
+        <v>135.13999999999999</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>135.60900000000001</v>
+      </c>
+      <c r="E94">
+        <v>1</v>
+      </c>
+      <c r="F94" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A91">
-        <v>1</v>
-      </c>
-      <c r="B91" t="str">
-        <f t="shared" si="2"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C91">
-        <v>131.85900000000001</v>
-      </c>
-      <c r="D91">
-        <v>0.8</v>
-      </c>
-      <c r="E91">
-        <v>133.26499999999999</v>
-      </c>
-      <c r="F91">
-        <v>0.8</v>
-      </c>
-      <c r="G91" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A92">
-        <v>1</v>
-      </c>
-      <c r="B92" t="str">
-        <f t="shared" si="2"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C92">
-        <v>133.26499999999999</v>
-      </c>
-      <c r="D92">
-        <v>0.8</v>
-      </c>
-      <c r="E92">
-        <v>133.73400000000001</v>
-      </c>
-      <c r="F92">
-        <v>0</v>
-      </c>
-      <c r="G92" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A93">
-        <v>1</v>
-      </c>
-      <c r="B93" t="str">
-        <f t="shared" si="2"/>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C93">
-        <v>133.73400000000001</v>
-      </c>
-      <c r="D93">
-        <v>0</v>
-      </c>
-      <c r="E93">
-        <v>135.13999999999999</v>
-      </c>
-      <c r="F93">
-        <v>0</v>
-      </c>
-      <c r="G93" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A94">
-        <v>1</v>
-      </c>
-      <c r="B94" t="str">
-        <f t="shared" ref="B94" si="3">VLOOKUP(A94,$I$1:$J$99,2,FALSE)</f>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C94">
-        <v>135.13999999999999</v>
-      </c>
-      <c r="D94">
-        <v>0</v>
-      </c>
-      <c r="E94">
-        <v>135.60900000000001</v>
-      </c>
-      <c r="F94">
-        <v>1</v>
-      </c>
-      <c r="G94" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>10</v>
       </c>
-      <c r="B95" t="str">
-        <f t="shared" ref="B95" si="4">VLOOKUP(A95,$I$1:$J$99,2,FALSE)</f>
-        <v>#f0ffff</v>
+      <c r="B95">
+        <v>135.13999999999999</v>
       </c>
       <c r="C95">
-        <v>135.13999999999999</v>
+        <v>0</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>138.88999999999999</v>
       </c>
       <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>1</v>
+      </c>
+      <c r="B96">
+        <v>135.60900000000001</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <v>137.01499999999999</v>
+      </c>
+      <c r="E96">
+        <v>1</v>
+      </c>
+      <c r="F96" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>1</v>
+      </c>
+      <c r="B97">
+        <v>137.01499999999999</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97">
         <v>138.88999999999999</v>
       </c>
-      <c r="F95">
-        <v>0</v>
-      </c>
-      <c r="G95" t="s">
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A96">
-        <v>1</v>
-      </c>
-      <c r="B96" t="str">
-        <f>VLOOKUP(A96,$I$1:$J$99,2,FALSE)</f>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C96">
-        <v>135.60900000000001</v>
-      </c>
-      <c r="D96">
-        <v>1</v>
-      </c>
-      <c r="E96">
-        <v>137.01499999999999</v>
-      </c>
-      <c r="F96">
-        <v>1</v>
-      </c>
-      <c r="G96" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A97">
-        <v>1</v>
-      </c>
-      <c r="B97" t="str">
-        <f t="shared" ref="B97" si="5">VLOOKUP(A97,$I$1:$J$99,2,FALSE)</f>
-        <v>#63b8ff</v>
-      </c>
-      <c r="C97">
-        <v>137.01499999999999</v>
-      </c>
-      <c r="D97">
-        <v>1</v>
-      </c>
-      <c r="E97">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>1</v>
+      </c>
+      <c r="B98">
         <v>138.88999999999999</v>
       </c>
-      <c r="F97">
-        <v>0</v>
-      </c>
-      <c r="G97" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A98">
-        <v>1</v>
-      </c>
-      <c r="B98" t="str">
-        <f t="shared" ref="B98" si="6">VLOOKUP(A98,$I$1:$J$99,2,FALSE)</f>
-        <v>#63b8ff</v>
-      </c>
       <c r="C98">
-        <v>138.88999999999999</v>
+        <v>0</v>
       </c>
       <c r="D98">
-        <v>0</v>
+        <v>154.828</v>
       </c>
       <c r="E98">
-        <v>154.828</v>
-      </c>
-      <c r="F98">
-        <v>0</v>
-      </c>
-      <c r="G98" t="s">
+        <v>0</v>
+      </c>
+      <c r="F98" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2990,7 +2613,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7059D0-50D6-42B0-899B-7876B4BEDB4C}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D668"/>
@@ -12360,13 +11983,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967B2D43-E0B0-4050-83A2-AF5C6E5EE029}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L200"/>
   <sheetViews>
-    <sheetView topLeftCell="A169" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C193" sqref="C193:E200"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -12403,7 +12026,7 @@
         <v>14</v>
       </c>
       <c r="K1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -19407,7 +19030,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C76DC57-EF49-44CE-8A21-D4353938F627}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:J62"/>
@@ -20346,12 +19969,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F96158-71D4-4C19-99F5-47E7932AF572}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
@@ -21854,13 +21477,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192095B2-1BEA-4365-B4DE-88EEBB6E4423}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
MultiHitLine effect, Star effect refine, and others..
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Songs/World Wide Web/Chart.xlsx
+++ b/Assets/StreamingAssets/Songs/World Wide Web/Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Xenody-master\Assets\StreamingAssets\Songs\World Wide Web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Xenody-main\Assets\StreamingAssets\Songs\World Wide Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F5EE69-EB4A-448F-8A13-261BCF7F1EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6252C739-5A9C-403D-9381-D95DE9A50C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="speed" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="36">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -154,6 +154,18 @@
   </si>
   <si>
     <t>sp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rad</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Angle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rot</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -577,7 +589,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75FB3F29-4751-4825-9A13-CD8F2FFC98B2}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D2"/>
     </sheetView>
   </sheetViews>
@@ -21480,15 +21492,15 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192095B2-1BEA-4365-B4DE-88EEBB6E4423}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -21518,6 +21530,15 @@
       </c>
       <c r="J1" t="s">
         <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add judge texture effect..
</commit_message>
<xml_diff>
--- a/Assets/StreamingAssets/Songs/World Wide Web/Chart.xlsx
+++ b/Assets/StreamingAssets/Songs/World Wide Web/Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Xenody-main\Assets\StreamingAssets\Songs\World Wide Web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Xenody-master\Assets\StreamingAssets\Songs\World Wide Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6252C739-5A9C-403D-9381-D95DE9A50C1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393E23CE-91BC-473E-AD78-E95349A5C597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" activeTab="1" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="speed" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="38">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -145,14 +145,6 @@
     <t>#f0ffff</t>
   </si>
   <si>
-    <t>Lcolor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ucolor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>sp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -166,6 +158,22 @@
   </si>
   <si>
     <t>Rot</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StartLcolor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StartUcolor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EndLcolor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EndUcolor</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -565,7 +573,7 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -587,15 +595,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75FB3F29-4751-4825-9A13-CD8F2FFC98B2}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -603,13 +611,19 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -21494,8 +21508,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -21532,13 +21546,13 @@
         <v>10</v>
       </c>
       <c r="K1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
         <v>33</v>
-      </c>
-      <c r="L1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>